<commit_message>
Add logistic regression script for next week
</commit_message>
<xml_diff>
--- a/data_raw/poisson_data.xlsx
+++ b/data_raw/poisson_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30257d98913de859/GitHub/cbc_coding_club/data_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30257d98913de859/Statistics/honours_course/tutorial_glm/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="8_{95181DCC-7BEC-414E-B64D-34D134BB5818}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E432A71E-0D72-4CD9-B37E-95F16FDE9FAF}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="8_{95181DCC-7BEC-414E-B64D-34D134BB5818}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B6981162-81D3-4FDA-8B14-83B6023C75EF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{481905D8-8826-4EB3-830D-DC998B182542}"/>
   </bookViews>
@@ -33,7 +33,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="8">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
   <si>
     <t>temp</t>
   </si>
@@ -398,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C185377-AFB5-4B67-9B9A-28F702485084}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -409,21 +421,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>15</v>
+      <c r="A2" t="s">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -436,8 +448,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>15</v>
+      <c r="A3" t="s">
+        <v>0</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -450,8 +462,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>15</v>
+      <c r="A4" t="s">
+        <v>0</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -464,8 +476,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>15</v>
+      <c r="A5" t="s">
+        <v>0</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -478,8 +490,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>15</v>
+      <c r="A6" t="s">
+        <v>0</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -492,8 +504,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>15</v>
+      <c r="A7" t="s">
+        <v>0</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -506,8 +518,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>15</v>
+      <c r="A8" t="s">
+        <v>0</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -520,8 +532,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>15</v>
+      <c r="A9" t="s">
+        <v>0</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -534,8 +546,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>15</v>
+      <c r="A10" t="s">
+        <v>0</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -548,8 +560,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>15</v>
+      <c r="A11" t="s">
+        <v>0</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -562,8 +574,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>15</v>
+      <c r="A12" t="s">
+        <v>0</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -576,8 +588,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>15</v>
+      <c r="A13" t="s">
+        <v>0</v>
       </c>
       <c r="B13">
         <v>7</v>
@@ -590,8 +602,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>15</v>
+      <c r="A14" t="s">
+        <v>0</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -604,8 +616,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>15</v>
+      <c r="A15" t="s">
+        <v>0</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -618,8 +630,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>0</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -632,8 +644,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>15</v>
+      <c r="A17" t="s">
+        <v>0</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -646,8 +658,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>15</v>
+      <c r="A18" t="s">
+        <v>0</v>
       </c>
       <c r="B18">
         <v>7</v>
@@ -660,8 +672,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>15</v>
+      <c r="A19" t="s">
+        <v>0</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -674,8 +686,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>15</v>
+      <c r="A20" t="s">
+        <v>0</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -688,8 +700,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>15</v>
+      <c r="A21" t="s">
+        <v>0</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -702,8 +714,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>20</v>
+      <c r="A22" t="s">
+        <v>1</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -716,8 +728,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>20</v>
+      <c r="A23" t="s">
+        <v>1</v>
       </c>
       <c r="B23">
         <v>6</v>
@@ -730,8 +742,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>20</v>
+      <c r="A24" t="s">
+        <v>1</v>
       </c>
       <c r="B24">
         <v>7</v>
@@ -744,8 +756,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>20</v>
+      <c r="A25" t="s">
+        <v>1</v>
       </c>
       <c r="B25">
         <v>8</v>
@@ -758,8 +770,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>20</v>
+      <c r="A26" t="s">
+        <v>1</v>
       </c>
       <c r="B26">
         <v>8</v>
@@ -772,8 +784,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>20</v>
+      <c r="A27" t="s">
+        <v>1</v>
       </c>
       <c r="B27">
         <v>5</v>
@@ -786,8 +798,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>20</v>
+      <c r="A28" t="s">
+        <v>1</v>
       </c>
       <c r="B28">
         <v>4</v>
@@ -800,8 +812,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>20</v>
+      <c r="A29" t="s">
+        <v>1</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -814,8 +826,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>20</v>
+      <c r="A30" t="s">
+        <v>1</v>
       </c>
       <c r="B30">
         <v>4</v>
@@ -828,8 +840,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>20</v>
+      <c r="A31" t="s">
+        <v>1</v>
       </c>
       <c r="B31">
         <v>6</v>
@@ -842,8 +854,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>20</v>
+      <c r="A32" t="s">
+        <v>1</v>
       </c>
       <c r="B32">
         <v>7</v>
@@ -856,8 +868,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>20</v>
+      <c r="A33" t="s">
+        <v>1</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -870,8 +882,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>20</v>
+      <c r="A34" t="s">
+        <v>1</v>
       </c>
       <c r="B34">
         <v>6</v>
@@ -884,8 +896,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>20</v>
+      <c r="A35" t="s">
+        <v>1</v>
       </c>
       <c r="B35">
         <v>5</v>
@@ -898,8 +910,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>20</v>
+      <c r="A36" t="s">
+        <v>1</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -912,8 +924,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>20</v>
+      <c r="A37" t="s">
+        <v>1</v>
       </c>
       <c r="B37">
         <v>6</v>
@@ -926,8 +938,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>20</v>
+      <c r="A38" t="s">
+        <v>1</v>
       </c>
       <c r="B38">
         <v>5</v>
@@ -940,8 +952,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>20</v>
+      <c r="A39" t="s">
+        <v>1</v>
       </c>
       <c r="B39">
         <v>7</v>
@@ -954,8 +966,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>20</v>
+      <c r="A40" t="s">
+        <v>1</v>
       </c>
       <c r="B40">
         <v>5</v>
@@ -968,8 +980,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>20</v>
+      <c r="A41" t="s">
+        <v>1</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -982,8 +994,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>25</v>
+      <c r="A42" t="s">
+        <v>2</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -996,8 +1008,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>25</v>
+      <c r="A43" t="s">
+        <v>2</v>
       </c>
       <c r="B43">
         <v>5</v>
@@ -1010,8 +1022,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>25</v>
+      <c r="A44" t="s">
+        <v>2</v>
       </c>
       <c r="B44">
         <v>6</v>
@@ -1024,8 +1036,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>25</v>
+      <c r="A45" t="s">
+        <v>2</v>
       </c>
       <c r="B45">
         <v>7</v>
@@ -1038,8 +1050,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <v>25</v>
+      <c r="A46" t="s">
+        <v>2</v>
       </c>
       <c r="B46">
         <v>8</v>
@@ -1052,8 +1064,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47">
-        <v>25</v>
+      <c r="A47" t="s">
+        <v>2</v>
       </c>
       <c r="B47">
         <v>8</v>
@@ -1066,8 +1078,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <v>25</v>
+      <c r="A48" t="s">
+        <v>2</v>
       </c>
       <c r="B48">
         <v>6</v>
@@ -1080,8 +1092,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>25</v>
+      <c r="A49" t="s">
+        <v>2</v>
       </c>
       <c r="B49">
         <v>5</v>
@@ -1094,8 +1106,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>25</v>
+      <c r="A50" t="s">
+        <v>2</v>
       </c>
       <c r="B50">
         <v>4</v>
@@ -1108,8 +1120,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <v>25</v>
+      <c r="A51" t="s">
+        <v>2</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -1122,8 +1134,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>25</v>
+      <c r="A52" t="s">
+        <v>2</v>
       </c>
       <c r="B52">
         <v>2</v>
@@ -1136,8 +1148,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>25</v>
+      <c r="A53" t="s">
+        <v>2</v>
       </c>
       <c r="B53">
         <v>3</v>
@@ -1150,8 +1162,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54">
-        <v>25</v>
+      <c r="A54" t="s">
+        <v>2</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -1164,8 +1176,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <v>25</v>
+      <c r="A55" t="s">
+        <v>2</v>
       </c>
       <c r="B55">
         <v>6</v>
@@ -1178,8 +1190,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <v>25</v>
+      <c r="A56" t="s">
+        <v>2</v>
       </c>
       <c r="B56">
         <v>7</v>
@@ -1192,8 +1204,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <v>25</v>
+      <c r="A57" t="s">
+        <v>2</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -1206,8 +1218,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <v>25</v>
+      <c r="A58" t="s">
+        <v>2</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -1220,8 +1232,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>25</v>
+      <c r="A59" t="s">
+        <v>2</v>
       </c>
       <c r="B59">
         <v>8</v>
@@ -1234,8 +1246,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>25</v>
+      <c r="A60" t="s">
+        <v>2</v>
       </c>
       <c r="B60">
         <v>4</v>
@@ -1248,8 +1260,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>25</v>
+      <c r="A61" t="s">
+        <v>2</v>
       </c>
       <c r="B61">
         <v>6</v>
@@ -1262,8 +1274,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>30</v>
+      <c r="A62" t="s">
+        <v>3</v>
       </c>
       <c r="B62">
         <v>5</v>
@@ -1276,8 +1288,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>30</v>
+      <c r="A63" t="s">
+        <v>3</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -1290,8 +1302,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>30</v>
+      <c r="A64" t="s">
+        <v>3</v>
       </c>
       <c r="B64">
         <v>4</v>
@@ -1304,8 +1316,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>30</v>
+      <c r="A65" t="s">
+        <v>3</v>
       </c>
       <c r="B65">
         <v>5</v>
@@ -1318,8 +1330,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>30</v>
+      <c r="A66" t="s">
+        <v>3</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -1332,8 +1344,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>30</v>
+      <c r="A67" t="s">
+        <v>3</v>
       </c>
       <c r="B67">
         <v>2</v>
@@ -1346,8 +1358,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>30</v>
+      <c r="A68" t="s">
+        <v>3</v>
       </c>
       <c r="B68">
         <v>4</v>
@@ -1360,8 +1372,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>30</v>
+      <c r="A69" t="s">
+        <v>3</v>
       </c>
       <c r="B69">
         <v>6</v>
@@ -1374,8 +1386,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>30</v>
+      <c r="A70" t="s">
+        <v>3</v>
       </c>
       <c r="B70">
         <v>7</v>
@@ -1388,8 +1400,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>30</v>
+      <c r="A71" t="s">
+        <v>3</v>
       </c>
       <c r="B71">
         <v>3</v>
@@ -1402,8 +1414,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>30</v>
+      <c r="A72" t="s">
+        <v>3</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -1416,8 +1428,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>30</v>
+      <c r="A73" t="s">
+        <v>3</v>
       </c>
       <c r="B73">
         <v>5</v>
@@ -1430,8 +1442,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <v>30</v>
+      <c r="A74" t="s">
+        <v>3</v>
       </c>
       <c r="B74">
         <v>7</v>
@@ -1444,8 +1456,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <v>30</v>
+      <c r="A75" t="s">
+        <v>3</v>
       </c>
       <c r="B75">
         <v>7</v>
@@ -1458,8 +1470,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <v>30</v>
+      <c r="A76" t="s">
+        <v>3</v>
       </c>
       <c r="B76">
         <v>7</v>
@@ -1472,8 +1484,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <v>30</v>
+      <c r="A77" t="s">
+        <v>3</v>
       </c>
       <c r="B77">
         <v>3</v>
@@ -1486,8 +1498,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>30</v>
+      <c r="A78" t="s">
+        <v>3</v>
       </c>
       <c r="B78">
         <v>4</v>
@@ -1500,8 +1512,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <v>30</v>
+      <c r="A79" t="s">
+        <v>3</v>
       </c>
       <c r="B79">
         <v>5</v>
@@ -1514,8 +1526,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80">
-        <v>30</v>
+      <c r="A80" t="s">
+        <v>3</v>
       </c>
       <c r="B80">
         <v>6</v>
@@ -1528,8 +1540,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81">
-        <v>30</v>
+      <c r="A81" t="s">
+        <v>3</v>
       </c>
       <c r="B81">
         <v>3</v>

</xml_diff>